<commit_message>
Updated API code for fetching equipments details from database to excel
</commit_message>
<xml_diff>
--- a/Equipments_details_file/venkateshtadpatri26@gmail.com-2025-11-25.xlsx
+++ b/Equipments_details_file/venkateshtadpatri26@gmail.com-2025-11-25.xlsx
@@ -53,7 +53,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
@@ -65,7 +65,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -510,156 +509,163 @@
       <c r="F1" s="3" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>FLOOR_1</t>
         </is>
       </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="B2" s="1" t="inlineStr">
         <is>
           <t>AC</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
+      <c r="C2" s="1" t="inlineStr">
         <is>
           <t>AC_1</t>
         </is>
       </c>
-      <c r="D2" s="5" t="n">
+      <c r="D2" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E2" s="5" t="inlineStr">
+      <c r="E2" s="1" t="inlineStr">
         <is>
           <t>Admin room</t>
         </is>
       </c>
+      <c r="F2" s="1" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>FLOOR_1</t>
         </is>
       </c>
-      <c r="B3" s="5" t="inlineStr">
+      <c r="B3" s="1" t="inlineStr">
         <is>
           <t>BATTERY</t>
         </is>
       </c>
-      <c r="C3" s="5" t="inlineStr">
+      <c r="C3" s="1" t="inlineStr">
         <is>
           <t>BATTERY_1</t>
         </is>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="E3" s="5" t="inlineStr">
+      <c r="E3" s="1" t="inlineStr">
         <is>
           <t>Conference</t>
         </is>
       </c>
+      <c r="F3" s="1" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>FLOOR_1</t>
         </is>
       </c>
-      <c r="B4" s="5" t="inlineStr">
+      <c r="B4" s="1" t="inlineStr">
         <is>
           <t>UPS</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr">
+      <c r="C4" s="1" t="inlineStr">
         <is>
           <t>UPS_1</t>
         </is>
       </c>
-      <c r="D4" s="5" t="n">
+      <c r="D4" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="E4" s="5" t="inlineStr">
+      <c r="E4" s="1" t="inlineStr">
         <is>
           <t>Conference</t>
         </is>
       </c>
+      <c r="F4" s="1" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="5" t="inlineStr">
+      <c r="A5" s="1" t="inlineStr">
         <is>
           <t>FLOOR_1</t>
         </is>
       </c>
-      <c r="B5" s="5" t="inlineStr">
+      <c r="B5" s="1" t="inlineStr">
         <is>
           <t>PANEL</t>
         </is>
       </c>
-      <c r="C5" s="5" t="inlineStr">
+      <c r="C5" s="1" t="inlineStr">
         <is>
           <t>PANEL_1</t>
         </is>
       </c>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="E5" s="5" t="inlineStr">
+      <c r="E5" s="1" t="inlineStr">
         <is>
           <t>Conference</t>
         </is>
       </c>
+      <c r="F5" s="1" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="5" t="inlineStr">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>FLOOR_1</t>
         </is>
       </c>
-      <c r="B6" s="5" t="inlineStr">
+      <c r="B6" s="1" t="inlineStr">
         <is>
           <t>SWITCHBOARD</t>
         </is>
       </c>
-      <c r="C6" s="5" t="inlineStr">
+      <c r="C6" s="1" t="inlineStr">
         <is>
           <t>SWITCH_2</t>
         </is>
       </c>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="E6" s="5" t="inlineStr">
+      <c r="E6" s="1" t="inlineStr">
         <is>
           <t>Conference</t>
         </is>
       </c>
+      <c r="F6" s="1" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="inlineStr">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>FLOOR_1</t>
         </is>
       </c>
-      <c r="B7" s="5" t="inlineStr">
+      <c r="B7" s="1" t="inlineStr">
         <is>
           <t>WIRING</t>
         </is>
       </c>
-      <c r="C7" s="5" t="inlineStr">
+      <c r="C7" s="1" t="inlineStr">
         <is>
           <t>WIRING_2</t>
         </is>
       </c>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="E7" s="5" t="inlineStr">
+      <c r="E7" s="1" t="inlineStr">
         <is>
           <t>Conference</t>
         </is>
       </c>
+      <c r="F7" s="1" t="n"/>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="0" selectUnlockedCells="0" algorithmName="SHA-512" sheet="1" objects="1" insertRows="1" insertHyperlinks="1" autoFilter="1" scenarios="1" formatColumns="1" deleteColumns="1" insertColumns="1" pivotTables="1" deleteRows="1" formatCells="1" saltValue="hT0htCEAUntJILJnC6942A==" formatRows="1" sort="1" spinCount="100000" hashValue="+1rJnNpO/LqPgizNMnKtGuPTYRbyCN6sUkPklhX8zp98JukDJ/TmvjpL+oNzW4CsVbJ/xHGAwMJQ1sZ9XH3sIA=="/>
   <dataValidations count="1">
     <dataValidation sqref="D1:D1048576" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="1" type="whole">
       <formula1>1</formula1>

</xml_diff>